<commit_message>
parlor's service implemenation and service edit done
</commit_message>
<xml_diff>
--- a/relatedFiles/other files/final/Services/services import list final to import.xlsx
+++ b/relatedFiles/other files/final/Services/services import list final to import.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Dev\Laravel\_Developing_Phase_Project\Murarkey Single Vendor\Murarkey_single_vendor_ecommerce_with_vuexy_template\relatedFiles\other files\Services\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\murarkey\Murarkey_single_vendor_ecommerce_with_vuexy_template\relatedFiles\other files\final\Services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049D8452-C254-42F8-BF5A-F5E534B04A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" forceFullCalc="1"/>
+  <calcPr calcId="162913" forceFullCalc="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="337">
   <si>
     <t>about</t>
   </si>
@@ -1164,16 +1163,19 @@
     <t>Slug</t>
   </si>
   <si>
-    <t>http://murarkey.com/image/cache/600X600/xc8H4rpAZTTlg9LrT0JXJf9rKAFMEFlXIayNAjTK.jpg</t>
-  </si>
-  <si>
     <t>https://cdn-icons-png.flaticon.com/512/3461/3461906.png</t>
+  </si>
+  <si>
+    <t>http://demo.murarkey.com/image/cache/600X600/xc8H4rpAZTTlg9LrT0JXJf9rKAFMEFlXIayNAjTK.jpg</t>
+  </si>
+  <si>
+    <t>https://demo.murarkey.com/image/cache/600X600/xc8H4rpAZTTlg9LrT0JXJf9rKAFMEFlXIayNAjTK.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1430,23 +1432,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1482,23 +1467,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1674,36 +1642,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M86" workbookViewId="0">
-      <selection activeCell="M99" sqref="M99"/>
+    <sheetView tabSelected="1" topLeftCell="N97" workbookViewId="0">
+      <selection activeCell="N81" sqref="N81:N107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="255.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="255.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="84.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="234.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="16.5703125" style="4"/>
+    <col min="5" max="5" width="40.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="255.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="255.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="84.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="234.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="16.5546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>117</v>
       </c>
@@ -1762,7 +1730,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>121</v>
       </c>
@@ -1801,10 +1769,10 @@
         <v>275</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O2" s="8" t="s">
         <v>116</v>
@@ -1819,7 +1787,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>121</v>
       </c>
@@ -1858,10 +1826,10 @@
         <v>276</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O3" s="8" t="s">
         <v>116</v>
@@ -1876,7 +1844,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>121</v>
       </c>
@@ -1915,10 +1883,10 @@
         <v>277</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O4" s="8" t="s">
         <v>116</v>
@@ -1933,7 +1901,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>121</v>
       </c>
@@ -1972,10 +1940,10 @@
         <v>277</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O5" s="8" t="s">
         <v>116</v>
@@ -1990,7 +1958,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>121</v>
       </c>
@@ -2029,10 +1997,10 @@
         <v>278</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O6" s="8" t="s">
         <v>116</v>
@@ -2047,7 +2015,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>121</v>
       </c>
@@ -2086,10 +2054,10 @@
         <v>279</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O7" s="8" t="s">
         <v>116</v>
@@ -2104,7 +2072,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>121</v>
       </c>
@@ -2143,10 +2111,10 @@
         <v>280</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O8" s="8" t="s">
         <v>116</v>
@@ -2161,7 +2129,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>121</v>
       </c>
@@ -2200,10 +2168,10 @@
         <v>281</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O9" s="8" t="s">
         <v>116</v>
@@ -2218,7 +2186,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>121</v>
       </c>
@@ -2257,10 +2225,10 @@
         <v>282</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O10" s="8" t="s">
         <v>116</v>
@@ -2275,7 +2243,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>121</v>
       </c>
@@ -2314,10 +2282,10 @@
         <v>283</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O11" s="8" t="s">
         <v>116</v>
@@ -2332,7 +2300,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>121</v>
       </c>
@@ -2371,10 +2339,10 @@
         <v>284</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O12" s="8" t="s">
         <v>116</v>
@@ -2389,7 +2357,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>121</v>
       </c>
@@ -2428,10 +2396,10 @@
         <v>285</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O13" s="8" t="s">
         <v>116</v>
@@ -2446,7 +2414,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>121</v>
       </c>
@@ -2485,10 +2453,10 @@
         <v>286</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O14" s="8" t="s">
         <v>116</v>
@@ -2503,7 +2471,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>121</v>
       </c>
@@ -2542,10 +2510,10 @@
         <v>287</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O15" s="8" t="s">
         <v>116</v>
@@ -2560,7 +2528,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>121</v>
       </c>
@@ -2599,10 +2567,10 @@
         <v>288</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O16" s="8" t="s">
         <v>116</v>
@@ -2617,7 +2585,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>121</v>
       </c>
@@ -2656,10 +2624,10 @@
         <v>289</v>
       </c>
       <c r="M17" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O17" s="8" t="s">
         <v>116</v>
@@ -2674,7 +2642,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>121</v>
       </c>
@@ -2713,10 +2681,10 @@
         <v>194</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O18" s="8" t="s">
         <v>116</v>
@@ -2731,7 +2699,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>121</v>
       </c>
@@ -2770,10 +2738,10 @@
         <v>290</v>
       </c>
       <c r="M19" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O19" s="8" t="s">
         <v>116</v>
@@ -2788,7 +2756,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>121</v>
       </c>
@@ -2827,10 +2795,10 @@
         <v>291</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O20" s="8" t="s">
         <v>116</v>
@@ -2845,7 +2813,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>120</v>
       </c>
@@ -2884,10 +2852,10 @@
         <v>277</v>
       </c>
       <c r="M21" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O21" s="8" t="s">
         <v>116</v>
@@ -2902,7 +2870,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>120</v>
       </c>
@@ -2941,10 +2909,10 @@
         <v>291</v>
       </c>
       <c r="M22" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O22" s="8" t="s">
         <v>116</v>
@@ -2959,7 +2927,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>120</v>
       </c>
@@ -2998,10 +2966,10 @@
         <v>278</v>
       </c>
       <c r="M23" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O23" s="8" t="s">
         <v>116</v>
@@ -3016,7 +2984,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>120</v>
       </c>
@@ -3055,10 +3023,10 @@
         <v>292</v>
       </c>
       <c r="M24" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O24" s="8" t="s">
         <v>116</v>
@@ -3073,7 +3041,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>120</v>
       </c>
@@ -3112,10 +3080,10 @@
         <v>293</v>
       </c>
       <c r="M25" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O25" s="8" t="s">
         <v>116</v>
@@ -3130,7 +3098,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>120</v>
       </c>
@@ -3169,10 +3137,10 @@
         <v>278</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O26" s="8" t="s">
         <v>116</v>
@@ -3187,7 +3155,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>120</v>
       </c>
@@ -3226,10 +3194,10 @@
         <v>294</v>
       </c>
       <c r="M27" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O27" s="8" t="s">
         <v>116</v>
@@ -3244,7 +3212,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>118</v>
       </c>
@@ -3283,10 +3251,10 @@
         <v>295</v>
       </c>
       <c r="M28" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O28" s="8" t="s">
         <v>116</v>
@@ -3301,7 +3269,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>118</v>
       </c>
@@ -3340,10 +3308,10 @@
         <v>296</v>
       </c>
       <c r="M29" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O29" s="8" t="s">
         <v>116</v>
@@ -3358,7 +3326,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>118</v>
       </c>
@@ -3397,10 +3365,10 @@
         <v>297</v>
       </c>
       <c r="M30" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N30" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O30" s="8" t="s">
         <v>116</v>
@@ -3415,7 +3383,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>118</v>
       </c>
@@ -3454,10 +3422,10 @@
         <v>298</v>
       </c>
       <c r="M31" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O31" s="8" t="s">
         <v>116</v>
@@ -3472,7 +3440,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>118</v>
       </c>
@@ -3511,10 +3479,10 @@
         <v>299</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O32" s="8" t="s">
         <v>116</v>
@@ -3529,7 +3497,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>118</v>
       </c>
@@ -3568,10 +3536,10 @@
         <v>300</v>
       </c>
       <c r="M33" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N33" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O33" s="8" t="s">
         <v>116</v>
@@ -3586,7 +3554,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>118</v>
       </c>
@@ -3625,10 +3593,10 @@
         <v>301</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N34" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O34" s="8" t="s">
         <v>116</v>
@@ -3643,7 +3611,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>118</v>
       </c>
@@ -3682,10 +3650,10 @@
         <v>302</v>
       </c>
       <c r="M35" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N35" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O35" s="8" t="s">
         <v>116</v>
@@ -3700,7 +3668,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>118</v>
       </c>
@@ -3739,10 +3707,10 @@
         <v>303</v>
       </c>
       <c r="M36" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N36" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O36" s="8" t="s">
         <v>116</v>
@@ -3757,7 +3725,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>118</v>
       </c>
@@ -3796,10 +3764,10 @@
         <v>304</v>
       </c>
       <c r="M37" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O37" s="8" t="s">
         <v>116</v>
@@ -3814,7 +3782,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>118</v>
       </c>
@@ -3853,10 +3821,10 @@
         <v>204</v>
       </c>
       <c r="M38" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N38" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O38" s="8" t="s">
         <v>116</v>
@@ -3871,7 +3839,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>118</v>
       </c>
@@ -3910,10 +3878,10 @@
         <v>305</v>
       </c>
       <c r="M39" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O39" s="8" t="s">
         <v>116</v>
@@ -3928,7 +3896,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>118</v>
       </c>
@@ -3967,10 +3935,10 @@
         <v>206</v>
       </c>
       <c r="M40" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N40" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O40" s="8" t="s">
         <v>116</v>
@@ -3985,7 +3953,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>118</v>
       </c>
@@ -4024,10 +3992,10 @@
         <v>207</v>
       </c>
       <c r="M41" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N41" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O41" s="8" t="s">
         <v>116</v>
@@ -4042,7 +4010,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>118</v>
       </c>
@@ -4078,10 +4046,10 @@
         <v>208</v>
       </c>
       <c r="M42" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N42" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O42" s="8" t="s">
         <v>116</v>
@@ -4096,7 +4064,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>118</v>
       </c>
@@ -4135,10 +4103,10 @@
         <v>209</v>
       </c>
       <c r="M43" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N43" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O43" s="8" t="s">
         <v>116</v>
@@ -4153,7 +4121,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>118</v>
       </c>
@@ -4192,10 +4160,10 @@
         <v>306</v>
       </c>
       <c r="M44" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N44" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O44" s="8" t="s">
         <v>116</v>
@@ -4210,7 +4178,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>118</v>
       </c>
@@ -4249,10 +4217,10 @@
         <v>307</v>
       </c>
       <c r="M45" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N45" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O45" s="8" t="s">
         <v>116</v>
@@ -4267,7 +4235,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>118</v>
       </c>
@@ -4306,10 +4274,10 @@
         <v>308</v>
       </c>
       <c r="M46" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N46" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O46" s="8" t="s">
         <v>116</v>
@@ -4324,7 +4292,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>118</v>
       </c>
@@ -4363,10 +4331,10 @@
         <v>210</v>
       </c>
       <c r="M47" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N47" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O47" s="8" t="s">
         <v>116</v>
@@ -4381,7 +4349,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>118</v>
       </c>
@@ -4420,10 +4388,10 @@
         <v>309</v>
       </c>
       <c r="M48" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N48" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O48" s="8" t="s">
         <v>116</v>
@@ -4438,7 +4406,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>118</v>
       </c>
@@ -4477,10 +4445,10 @@
         <v>284</v>
       </c>
       <c r="M49" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N49" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O49" s="8" t="s">
         <v>116</v>
@@ -4495,7 +4463,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>118</v>
       </c>
@@ -4534,10 +4502,10 @@
         <v>310</v>
       </c>
       <c r="M50" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N50" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O50" s="8" t="s">
         <v>116</v>
@@ -4552,7 +4520,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>118</v>
       </c>
@@ -4591,10 +4559,10 @@
         <v>311</v>
       </c>
       <c r="M51" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N51" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O51" s="8" t="s">
         <v>116</v>
@@ -4609,7 +4577,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>118</v>
       </c>
@@ -4648,10 +4616,10 @@
         <v>311</v>
       </c>
       <c r="M52" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N52" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O52" s="8" t="s">
         <v>116</v>
@@ -4666,7 +4634,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>118</v>
       </c>
@@ -4705,10 +4673,10 @@
         <v>311</v>
       </c>
       <c r="M53" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N53" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O53" s="8" t="s">
         <v>116</v>
@@ -4723,7 +4691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>118</v>
       </c>
@@ -4762,10 +4730,10 @@
         <v>297</v>
       </c>
       <c r="M54" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N54" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O54" s="8" t="s">
         <v>116</v>
@@ -4780,7 +4748,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>118</v>
       </c>
@@ -4819,10 +4787,10 @@
         <v>297</v>
       </c>
       <c r="M55" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N55" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O55" s="8" t="s">
         <v>116</v>
@@ -4837,7 +4805,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>118</v>
       </c>
@@ -4876,10 +4844,10 @@
         <v>312</v>
       </c>
       <c r="M56" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N56" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O56" s="8" t="s">
         <v>116</v>
@@ -4894,7 +4862,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>118</v>
       </c>
@@ -4933,10 +4901,10 @@
         <v>312</v>
       </c>
       <c r="M57" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N57" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O57" s="8" t="s">
         <v>116</v>
@@ -4951,7 +4919,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>118</v>
       </c>
@@ -4990,10 +4958,10 @@
         <v>215</v>
       </c>
       <c r="M58" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N58" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O58" s="8" t="s">
         <v>116</v>
@@ -5008,7 +4976,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>118</v>
       </c>
@@ -5047,10 +5015,10 @@
         <v>216</v>
       </c>
       <c r="M59" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N59" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O59" s="8" t="s">
         <v>116</v>
@@ -5065,7 +5033,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>118</v>
       </c>
@@ -5104,10 +5072,10 @@
         <v>306</v>
       </c>
       <c r="M60" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N60" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O60" s="8" t="s">
         <v>116</v>
@@ -5122,7 +5090,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>118</v>
       </c>
@@ -5161,10 +5129,10 @@
         <v>279</v>
       </c>
       <c r="M61" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N61" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O61" s="8" t="s">
         <v>116</v>
@@ -5179,7 +5147,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>118</v>
       </c>
@@ -5218,10 +5186,10 @@
         <v>217</v>
       </c>
       <c r="M62" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N62" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O62" s="8" t="s">
         <v>116</v>
@@ -5236,7 +5204,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>118</v>
       </c>
@@ -5275,10 +5243,10 @@
         <v>313</v>
       </c>
       <c r="M63" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N63" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O63" s="8" t="s">
         <v>116</v>
@@ -5293,7 +5261,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>118</v>
       </c>
@@ -5332,10 +5300,10 @@
         <v>314</v>
       </c>
       <c r="M64" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N64" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O64" s="8" t="s">
         <v>116</v>
@@ -5350,7 +5318,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>118</v>
       </c>
@@ -5389,10 +5357,10 @@
         <v>292</v>
       </c>
       <c r="M65" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N65" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O65" s="8" t="s">
         <v>116</v>
@@ -5407,7 +5375,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>118</v>
       </c>
@@ -5446,10 +5414,10 @@
         <v>315</v>
       </c>
       <c r="M66" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N66" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O66" s="8" t="s">
         <v>116</v>
@@ -5464,7 +5432,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>118</v>
       </c>
@@ -5503,10 +5471,10 @@
         <v>312</v>
       </c>
       <c r="M67" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N67" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O67" s="8" t="s">
         <v>116</v>
@@ -5521,7 +5489,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>118</v>
       </c>
@@ -5560,10 +5528,10 @@
         <v>312</v>
       </c>
       <c r="M68" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N68" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O68" s="8" t="s">
         <v>116</v>
@@ -5578,7 +5546,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>118</v>
       </c>
@@ -5617,10 +5585,10 @@
         <v>312</v>
       </c>
       <c r="M69" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N69" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O69" s="8" t="s">
         <v>116</v>
@@ -5635,7 +5603,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>118</v>
       </c>
@@ -5674,10 +5642,10 @@
         <v>312</v>
       </c>
       <c r="M70" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N70" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O70" s="8" t="s">
         <v>116</v>
@@ -5692,7 +5660,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>118</v>
       </c>
@@ -5731,10 +5699,10 @@
         <v>311</v>
       </c>
       <c r="M71" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N71" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O71" s="8" t="s">
         <v>116</v>
@@ -5749,7 +5717,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>118</v>
       </c>
@@ -5788,10 +5756,10 @@
         <v>220</v>
       </c>
       <c r="M72" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N72" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O72" s="8" t="s">
         <v>116</v>
@@ -5806,7 +5774,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>118</v>
       </c>
@@ -5845,10 +5813,10 @@
         <v>221</v>
       </c>
       <c r="M73" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N73" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O73" s="8" t="s">
         <v>116</v>
@@ -5863,7 +5831,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>118</v>
       </c>
@@ -5902,10 +5870,10 @@
         <v>222</v>
       </c>
       <c r="M74" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N74" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O74" s="8" t="s">
         <v>116</v>
@@ -5920,7 +5888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>118</v>
       </c>
@@ -5959,10 +5927,10 @@
         <v>282</v>
       </c>
       <c r="M75" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N75" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O75" s="8" t="s">
         <v>116</v>
@@ -5977,7 +5945,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>118</v>
       </c>
@@ -6016,10 +5984,10 @@
         <v>316</v>
       </c>
       <c r="M76" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N76" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O76" s="8" t="s">
         <v>116</v>
@@ -6034,7 +6002,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>118</v>
       </c>
@@ -6073,10 +6041,10 @@
         <v>317</v>
       </c>
       <c r="M77" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N77" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O77" s="8" t="s">
         <v>116</v>
@@ -6091,7 +6059,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>118</v>
       </c>
@@ -6130,10 +6098,10 @@
         <v>318</v>
       </c>
       <c r="M78" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N78" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O78" s="8" t="s">
         <v>116</v>
@@ -6148,7 +6116,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>119</v>
       </c>
@@ -6187,10 +6155,10 @@
         <v>319</v>
       </c>
       <c r="M79" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N79" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O79" s="8" t="s">
         <v>116</v>
@@ -6205,7 +6173,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>119</v>
       </c>
@@ -6244,10 +6212,10 @@
         <v>224</v>
       </c>
       <c r="M80" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N80" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O80" s="8" t="s">
         <v>116</v>
@@ -6262,7 +6230,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>119</v>
       </c>
@@ -6301,10 +6269,10 @@
         <v>224</v>
       </c>
       <c r="M81" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N81" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O81" s="8" t="s">
         <v>116</v>
@@ -6319,7 +6287,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>119</v>
       </c>
@@ -6358,10 +6326,10 @@
         <v>225</v>
       </c>
       <c r="M82" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N82" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O82" s="8" t="s">
         <v>116</v>
@@ -6376,7 +6344,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>119</v>
       </c>
@@ -6415,10 +6383,10 @@
         <v>226</v>
       </c>
       <c r="M83" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N83" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O83" s="8" t="s">
         <v>116</v>
@@ -6433,7 +6401,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>119</v>
       </c>
@@ -6472,10 +6440,10 @@
         <v>320</v>
       </c>
       <c r="M84" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N84" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O84" s="8" t="s">
         <v>116</v>
@@ -6490,7 +6458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>119</v>
       </c>
@@ -6529,10 +6497,10 @@
         <v>321</v>
       </c>
       <c r="M85" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N85" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O85" s="8" t="s">
         <v>116</v>
@@ -6547,7 +6515,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>119</v>
       </c>
@@ -6586,10 +6554,10 @@
         <v>322</v>
       </c>
       <c r="M86" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N86" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O86" s="8" t="s">
         <v>116</v>
@@ -6604,7 +6572,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>119</v>
       </c>
@@ -6643,10 +6611,10 @@
         <v>228</v>
       </c>
       <c r="M87" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N87" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O87" s="8" t="s">
         <v>116</v>
@@ -6661,7 +6629,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>119</v>
       </c>
@@ -6700,10 +6668,10 @@
         <v>323</v>
       </c>
       <c r="M88" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N88" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O88" s="8" t="s">
         <v>116</v>
@@ -6718,7 +6686,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>119</v>
       </c>
@@ -6757,10 +6725,10 @@
         <v>324</v>
       </c>
       <c r="M89" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N89" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O89" s="8" t="s">
         <v>116</v>
@@ -6775,7 +6743,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>119</v>
       </c>
@@ -6814,10 +6782,10 @@
         <v>325</v>
       </c>
       <c r="M90" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N90" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O90" s="8" t="s">
         <v>116</v>
@@ -6832,7 +6800,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>119</v>
       </c>
@@ -6871,10 +6839,10 @@
         <v>326</v>
       </c>
       <c r="M91" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N91" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O91" s="8" t="s">
         <v>116</v>
@@ -6889,7 +6857,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>119</v>
       </c>
@@ -6928,10 +6896,10 @@
         <v>327</v>
       </c>
       <c r="M92" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N92" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O92" s="8" t="s">
         <v>116</v>
@@ -6946,7 +6914,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>119</v>
       </c>
@@ -6985,10 +6953,10 @@
         <v>230</v>
       </c>
       <c r="M93" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N93" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O93" s="8" t="s">
         <v>116</v>
@@ -7003,7 +6971,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>119</v>
       </c>
@@ -7042,10 +7010,10 @@
         <v>328</v>
       </c>
       <c r="M94" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N94" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O94" s="8" t="s">
         <v>116</v>
@@ -7060,7 +7028,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
         <v>119</v>
       </c>
@@ -7099,10 +7067,10 @@
         <v>329</v>
       </c>
       <c r="M95" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N95" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O95" s="8" t="s">
         <v>116</v>
@@ -7117,7 +7085,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>119</v>
       </c>
@@ -7156,10 +7124,10 @@
         <v>224</v>
       </c>
       <c r="M96" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N96" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O96" s="8" t="s">
         <v>116</v>
@@ -7174,7 +7142,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>119</v>
       </c>
@@ -7213,10 +7181,10 @@
         <v>232</v>
       </c>
       <c r="M97" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N97" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O97" s="8" t="s">
         <v>116</v>
@@ -7231,7 +7199,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>119</v>
       </c>
@@ -7270,10 +7238,10 @@
         <v>233</v>
       </c>
       <c r="M98" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N98" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O98" s="8" t="s">
         <v>116</v>
@@ -7288,7 +7256,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>119</v>
       </c>
@@ -7327,10 +7295,10 @@
         <v>234</v>
       </c>
       <c r="M99" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N99" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O99" s="8" t="s">
         <v>116</v>
@@ -7345,7 +7313,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
         <v>119</v>
       </c>
@@ -7384,10 +7352,10 @@
         <v>330</v>
       </c>
       <c r="M100" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N100" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O100" s="8" t="s">
         <v>116</v>
@@ -7402,7 +7370,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>119</v>
       </c>
@@ -7441,10 +7409,10 @@
         <v>330</v>
       </c>
       <c r="M101" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N101" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O101" s="8" t="s">
         <v>116</v>
@@ -7459,7 +7427,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
         <v>119</v>
       </c>
@@ -7498,10 +7466,10 @@
         <v>331</v>
       </c>
       <c r="M102" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N102" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O102" s="8" t="s">
         <v>116</v>
@@ -7516,7 +7484,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>119</v>
       </c>
@@ -7555,10 +7523,10 @@
         <v>332</v>
       </c>
       <c r="M103" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N103" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O103" s="8" t="s">
         <v>116</v>
@@ -7573,7 +7541,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>119</v>
       </c>
@@ -7612,10 +7580,10 @@
         <v>238</v>
       </c>
       <c r="M104" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N104" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O104" s="8" t="s">
         <v>116</v>
@@ -7630,7 +7598,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>119</v>
       </c>
@@ -7669,10 +7637,10 @@
         <v>208</v>
       </c>
       <c r="M105" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N105" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O105" s="8" t="s">
         <v>116</v>
@@ -7687,7 +7655,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>119</v>
       </c>
@@ -7726,10 +7694,10 @@
         <v>239</v>
       </c>
       <c r="M106" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N106" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O106" s="8" t="s">
         <v>116</v>
@@ -7744,7 +7712,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>119</v>
       </c>
@@ -7783,10 +7751,10 @@
         <v>291</v>
       </c>
       <c r="M107" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N107" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="O107" s="8" t="s">
         <v>116</v>
@@ -7801,17 +7769,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B108" s="10"/>
+      <c r="N108" s="9"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S107">
+  <sortState ref="A2:S107">
     <sortCondition ref="A2:A107"/>
     <sortCondition ref="B2:B107"/>
     <sortCondition ref="C2:C107"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="M2" r:id="rId1"/>
+    <hyperlink ref="N2" r:id="rId2"/>
+    <hyperlink ref="N81" r:id="rId3"/>
+    <hyperlink ref="N82:N107" r:id="rId4" display="https://demo.murarkey.com/image/cache/600X600/xc8H4rpAZTTlg9LrT0JXJf9rKAFMEFlXIayNAjTK.jpg"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>